<commit_message>
emproloijo base de datos
</commit_message>
<xml_diff>
--- a/Fuentes/gabinete_fernandez.xlsx
+++ b/Fuentes/gabinete_fernandez.xlsx
@@ -5,18 +5,17 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\capacitacionazp1\Downloads\Gabinete  Fernandez-20191209T125537Z-001\Gabinete  Fernandez\gabinete_fernandez\Fuentes\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\capacitacionazp1\Downloads\gabinete\gabinete_fernandez\Fuentes\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6930"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6930" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Fernandez_datos" sheetId="1" r:id="rId1"/>
     <sheet name="fernandes_fuente" sheetId="2" r:id="rId2"/>
     <sheet name="Macri_datos" sheetId="3" r:id="rId3"/>
     <sheet name="Macri_fuente" sheetId="4" r:id="rId4"/>
-    <sheet name="consolidado" sheetId="5" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Fernandez_datos!$A$2:$H$34</definedName>
@@ -31,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="781" uniqueCount="184">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="459" uniqueCount="182">
   <si>
     <t>Wado de Pedro</t>
   </si>
@@ -574,12 +573,6 @@
   </si>
   <si>
     <t>edad_2015</t>
-  </si>
-  <si>
-    <t>Juntos por el Cambio</t>
-  </si>
-  <si>
-    <t>Frente de Todxs}</t>
   </si>
   <si>
     <t>Sin dato</t>
@@ -912,15 +905,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr filterMode="1"/>
   <dimension ref="A2:I34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+    <sheetView topLeftCell="A2" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection activeCell="A2" sqref="A2"/>
       <selection pane="topRight" activeCell="C2" sqref="C2"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="E5" sqref="E5"/>
+      <selection pane="bottomRight" activeCell="A2" sqref="A2:H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1011,7 +1003,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="5" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -1025,10 +1017,10 @@
         <v>60</v>
       </c>
       <c r="E5" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="F5" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="G5" t="s">
         <v>96</v>
@@ -1086,7 +1078,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="8" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>75</v>
       </c>
@@ -1112,7 +1104,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="9" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>44</v>
       </c>
@@ -1141,7 +1133,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>10</v>
       </c>
@@ -1297,7 +1289,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="16" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>19</v>
       </c>
@@ -1349,7 +1341,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="18" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>23</v>
       </c>
@@ -1404,7 +1396,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="20" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>25</v>
       </c>
@@ -1433,7 +1425,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:9" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>56</v>
       </c>
@@ -1462,7 +1454,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:9" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>27</v>
       </c>
@@ -1491,7 +1483,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>81</v>
       </c>
@@ -1520,7 +1512,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:9" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>30</v>
       </c>
@@ -1549,7 +1541,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>32</v>
       </c>
@@ -1575,7 +1567,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="26" spans="1:9" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>80</v>
       </c>
@@ -1601,7 +1593,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="27" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>35</v>
       </c>
@@ -1627,7 +1619,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="28" spans="1:9" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>36</v>
       </c>
@@ -1679,7 +1671,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="30" spans="1:9" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>39</v>
       </c>
@@ -1708,7 +1700,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>41</v>
       </c>
@@ -1737,7 +1729,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:9" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>58</v>
       </c>
@@ -1757,13 +1749,13 @@
         <v>77</v>
       </c>
       <c r="G32" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="I32">
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>49</v>
       </c>
@@ -1789,7 +1781,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="34" spans="1:9" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>51</v>
       </c>
@@ -1819,13 +1811,6 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A2:H34">
-    <filterColumn colId="2">
-      <filters>
-        <filter val="Abogacía"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -1873,7 +1858,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I31"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
@@ -2311,7 +2296,7 @@
         <v>134</v>
       </c>
       <c r="C15" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="D15">
         <v>50</v>
@@ -2701,7 +2686,7 @@
         <v>52</v>
       </c>
       <c r="C28" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="E28" t="s">
         <v>61</v>
@@ -2724,7 +2709,7 @@
         <v>15</v>
       </c>
       <c r="C29" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="E29" t="s">
         <v>60</v>
@@ -2747,7 +2732,7 @@
         <v>46</v>
       </c>
       <c r="C30" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="D30">
         <v>52</v>
@@ -2777,19 +2762,19 @@
         <v>8</v>
       </c>
       <c r="C31" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="E31" t="s">
         <v>60</v>
       </c>
       <c r="F31" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="G31" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="H31" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
   </sheetData>
@@ -2805,7 +2790,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -2824,1240 +2809,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J63"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A28" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B34" sqref="B34"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="24.453125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="45" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.7265625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" t="s">
-        <v>60</v>
-      </c>
-      <c r="E2" t="s">
-        <v>73</v>
-      </c>
-      <c r="F2" t="s">
-        <v>77</v>
-      </c>
-      <c r="G2" t="s">
-        <v>96</v>
-      </c>
-      <c r="H2">
-        <v>43</v>
-      </c>
-      <c r="J2" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D3" t="s">
-        <v>60</v>
-      </c>
-      <c r="E3" t="s">
-        <v>73</v>
-      </c>
-      <c r="F3" t="s">
-        <v>77</v>
-      </c>
-      <c r="G3" t="s">
-        <v>97</v>
-      </c>
-      <c r="H3">
-        <v>60</v>
-      </c>
-      <c r="J3" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" t="s">
-        <v>65</v>
-      </c>
-      <c r="D4" t="s">
-        <v>60</v>
-      </c>
-      <c r="G4" t="s">
-        <v>96</v>
-      </c>
-      <c r="H4">
-        <v>54</v>
-      </c>
-      <c r="J4" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5" t="s">
-        <v>1</v>
-      </c>
-      <c r="D5" t="s">
-        <v>61</v>
-      </c>
-      <c r="E5" t="s">
-        <v>73</v>
-      </c>
-      <c r="F5" t="s">
-        <v>77</v>
-      </c>
-      <c r="G5" t="s">
-        <v>97</v>
-      </c>
-      <c r="H5">
-        <v>42</v>
-      </c>
-      <c r="J5" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" t="s">
-        <v>42</v>
-      </c>
-      <c r="C6" t="s">
-        <v>1</v>
-      </c>
-      <c r="D6" t="s">
-        <v>60</v>
-      </c>
-      <c r="E6" t="s">
-        <v>73</v>
-      </c>
-      <c r="F6" t="s">
-        <v>77</v>
-      </c>
-      <c r="G6" t="s">
-        <v>97</v>
-      </c>
-      <c r="J6" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
-        <v>75</v>
-      </c>
-      <c r="B7" t="s">
-        <v>43</v>
-      </c>
-      <c r="C7" t="s">
-        <v>111</v>
-      </c>
-      <c r="D7" t="s">
-        <v>60</v>
-      </c>
-      <c r="E7" t="s">
-        <v>76</v>
-      </c>
-      <c r="F7" t="s">
-        <v>77</v>
-      </c>
-      <c r="G7" t="s">
-        <v>100</v>
-      </c>
-      <c r="H7">
-        <v>61</v>
-      </c>
-      <c r="J7" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
-        <v>44</v>
-      </c>
-      <c r="B8" t="s">
-        <v>45</v>
-      </c>
-      <c r="C8" t="s">
-        <v>72</v>
-      </c>
-      <c r="D8" t="s">
-        <v>60</v>
-      </c>
-      <c r="E8" t="s">
-        <v>78</v>
-      </c>
-      <c r="F8" t="s">
-        <v>77</v>
-      </c>
-      <c r="G8" t="s">
-        <v>97</v>
-      </c>
-      <c r="H8">
-        <v>41</v>
-      </c>
-      <c r="I8">
-        <v>1</v>
-      </c>
-      <c r="J8" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
-        <v>10</v>
-      </c>
-      <c r="B9" t="s">
-        <v>11</v>
-      </c>
-      <c r="C9" t="s">
-        <v>64</v>
-      </c>
-      <c r="D9" t="s">
-        <v>60</v>
-      </c>
-      <c r="E9" t="s">
-        <v>73</v>
-      </c>
-      <c r="F9" t="s">
-        <v>77</v>
-      </c>
-      <c r="G9" t="s">
-        <v>97</v>
-      </c>
-      <c r="H9">
-        <v>67</v>
-      </c>
-      <c r="J9" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
-        <v>47</v>
-      </c>
-      <c r="B10" t="s">
-        <v>46</v>
-      </c>
-      <c r="C10" t="s">
-        <v>1</v>
-      </c>
-      <c r="D10" t="s">
-        <v>60</v>
-      </c>
-      <c r="E10" t="s">
-        <v>85</v>
-      </c>
-      <c r="F10" t="s">
-        <v>77</v>
-      </c>
-      <c r="G10" t="s">
-        <v>102</v>
-      </c>
-      <c r="H10">
-        <v>65</v>
-      </c>
-      <c r="J10" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
-        <v>12</v>
-      </c>
-      <c r="B11" t="s">
-        <v>13</v>
-      </c>
-      <c r="C11" t="s">
-        <v>1</v>
-      </c>
-      <c r="D11" t="s">
-        <v>61</v>
-      </c>
-      <c r="E11" t="s">
-        <v>73</v>
-      </c>
-      <c r="F11" t="s">
-        <v>77</v>
-      </c>
-      <c r="G11" t="s">
-        <v>95</v>
-      </c>
-      <c r="H11">
-        <v>59</v>
-      </c>
-      <c r="J11" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A12" t="s">
-        <v>14</v>
-      </c>
-      <c r="B12" t="s">
-        <v>15</v>
-      </c>
-      <c r="C12" t="s">
-        <v>1</v>
-      </c>
-      <c r="D12" t="s">
-        <v>60</v>
-      </c>
-      <c r="E12" t="s">
-        <v>73</v>
-      </c>
-      <c r="F12" t="s">
-        <v>77</v>
-      </c>
-      <c r="G12" t="s">
-        <v>97</v>
-      </c>
-      <c r="H12">
-        <v>57</v>
-      </c>
-      <c r="J12" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A13" t="s">
-        <v>16</v>
-      </c>
-      <c r="B13" t="s">
-        <v>17</v>
-      </c>
-      <c r="C13" t="s">
-        <v>1</v>
-      </c>
-      <c r="D13" t="s">
-        <v>60</v>
-      </c>
-      <c r="E13" t="s">
-        <v>73</v>
-      </c>
-      <c r="F13" t="s">
-        <v>77</v>
-      </c>
-      <c r="G13" t="s">
-        <v>97</v>
-      </c>
-      <c r="H13">
-        <v>39</v>
-      </c>
-      <c r="J13" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A14" t="s">
-        <v>18</v>
-      </c>
-      <c r="B14" t="s">
-        <v>48</v>
-      </c>
-      <c r="C14" t="s">
-        <v>1</v>
-      </c>
-      <c r="D14" t="s">
-        <v>61</v>
-      </c>
-      <c r="E14" t="s">
-        <v>73</v>
-      </c>
-      <c r="F14" t="s">
-        <v>77</v>
-      </c>
-      <c r="G14" t="s">
-        <v>97</v>
-      </c>
-      <c r="H14">
-        <v>61</v>
-      </c>
-      <c r="J14" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A15" t="s">
-        <v>19</v>
-      </c>
-      <c r="B15" t="s">
-        <v>20</v>
-      </c>
-      <c r="C15" t="s">
-        <v>62</v>
-      </c>
-      <c r="D15" t="s">
-        <v>60</v>
-      </c>
-      <c r="E15" t="s">
-        <v>101</v>
-      </c>
-      <c r="F15" t="s">
-        <v>77</v>
-      </c>
-      <c r="G15" t="s">
-        <v>96</v>
-      </c>
-      <c r="H15">
-        <v>60</v>
-      </c>
-      <c r="J15" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A16" t="s">
-        <v>21</v>
-      </c>
-      <c r="B16" t="s">
-        <v>22</v>
-      </c>
-      <c r="C16" t="s">
-        <v>1</v>
-      </c>
-      <c r="D16" t="s">
-        <v>60</v>
-      </c>
-      <c r="E16" t="s">
-        <v>83</v>
-      </c>
-      <c r="F16" t="s">
-        <v>84</v>
-      </c>
-      <c r="G16" t="s">
-        <v>97</v>
-      </c>
-      <c r="H16">
-        <v>43</v>
-      </c>
-      <c r="J16" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A17" t="s">
-        <v>23</v>
-      </c>
-      <c r="B17" t="s">
-        <v>24</v>
-      </c>
-      <c r="C17" t="s">
-        <v>69</v>
-      </c>
-      <c r="D17" t="s">
-        <v>60</v>
-      </c>
-      <c r="E17" t="s">
-        <v>73</v>
-      </c>
-      <c r="F17" t="s">
-        <v>77</v>
-      </c>
-      <c r="G17" t="s">
-        <v>95</v>
-      </c>
-      <c r="H17">
-        <v>53</v>
-      </c>
-      <c r="I17">
-        <v>1</v>
-      </c>
-      <c r="J17" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A18" t="s">
-        <v>53</v>
-      </c>
-      <c r="B18" t="s">
-        <v>54</v>
-      </c>
-      <c r="C18" t="s">
-        <v>1</v>
-      </c>
-      <c r="D18" t="s">
-        <v>61</v>
-      </c>
-      <c r="E18" t="s">
-        <v>73</v>
-      </c>
-      <c r="F18" t="s">
-        <v>77</v>
-      </c>
-      <c r="G18" t="s">
-        <v>95</v>
-      </c>
-      <c r="H18">
-        <v>47</v>
-      </c>
-      <c r="J18" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A19" t="s">
-        <v>25</v>
-      </c>
-      <c r="B19" t="s">
-        <v>55</v>
-      </c>
-      <c r="C19" t="s">
-        <v>63</v>
-      </c>
-      <c r="D19" t="s">
-        <v>60</v>
-      </c>
-      <c r="E19" t="s">
-        <v>73</v>
-      </c>
-      <c r="F19" t="s">
-        <v>77</v>
-      </c>
-      <c r="G19" t="s">
-        <v>97</v>
-      </c>
-      <c r="H19">
-        <v>47</v>
-      </c>
-      <c r="I19">
-        <v>1</v>
-      </c>
-      <c r="J19" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A20" t="s">
-        <v>56</v>
-      </c>
-      <c r="B20" t="s">
-        <v>26</v>
-      </c>
-      <c r="C20" t="s">
-        <v>63</v>
-      </c>
-      <c r="D20" t="s">
-        <v>61</v>
-      </c>
-      <c r="E20" t="s">
-        <v>73</v>
-      </c>
-      <c r="F20" t="s">
-        <v>77</v>
-      </c>
-      <c r="G20" t="s">
-        <v>97</v>
-      </c>
-      <c r="H20">
-        <v>60</v>
-      </c>
-      <c r="I20">
-        <v>1</v>
-      </c>
-      <c r="J20" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A21" t="s">
-        <v>27</v>
-      </c>
-      <c r="B21" t="s">
-        <v>28</v>
-      </c>
-      <c r="C21" t="s">
-        <v>69</v>
-      </c>
-      <c r="D21" t="s">
-        <v>61</v>
-      </c>
-      <c r="E21" t="s">
-        <v>73</v>
-      </c>
-      <c r="F21" t="s">
-        <v>77</v>
-      </c>
-      <c r="G21" t="s">
-        <v>103</v>
-      </c>
-      <c r="H21">
-        <v>40</v>
-      </c>
-      <c r="I21">
-        <v>1</v>
-      </c>
-      <c r="J21" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A22" t="s">
-        <v>81</v>
-      </c>
-      <c r="B22" t="s">
-        <v>29</v>
-      </c>
-      <c r="C22" t="s">
-        <v>63</v>
-      </c>
-      <c r="D22" t="s">
-        <v>60</v>
-      </c>
-      <c r="E22" t="s">
-        <v>82</v>
-      </c>
-      <c r="F22" t="s">
-        <v>77</v>
-      </c>
-      <c r="G22" t="s">
-        <v>99</v>
-      </c>
-      <c r="H22">
-        <v>37</v>
-      </c>
-      <c r="I22">
-        <v>1</v>
-      </c>
-      <c r="J22" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A23" t="s">
-        <v>30</v>
-      </c>
-      <c r="B23" t="s">
-        <v>31</v>
-      </c>
-      <c r="C23" t="s">
-        <v>66</v>
-      </c>
-      <c r="D23" t="s">
-        <v>61</v>
-      </c>
-      <c r="E23" t="s">
-        <v>73</v>
-      </c>
-      <c r="F23" t="s">
-        <v>77</v>
-      </c>
-      <c r="G23" t="s">
-        <v>95</v>
-      </c>
-      <c r="H23">
-        <v>54</v>
-      </c>
-      <c r="I23">
-        <v>1</v>
-      </c>
-      <c r="J23" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A24" t="s">
-        <v>32</v>
-      </c>
-      <c r="B24" t="s">
-        <v>33</v>
-      </c>
-      <c r="C24" t="s">
-        <v>67</v>
-      </c>
-      <c r="D24" t="s">
-        <v>60</v>
-      </c>
-      <c r="E24" t="s">
-        <v>85</v>
-      </c>
-      <c r="F24" t="s">
-        <v>77</v>
-      </c>
-      <c r="G24" t="s">
-        <v>96</v>
-      </c>
-      <c r="H24">
-        <v>74</v>
-      </c>
-      <c r="J24" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A25" t="s">
-        <v>80</v>
-      </c>
-      <c r="B25" t="s">
-        <v>34</v>
-      </c>
-      <c r="C25" t="s">
-        <v>68</v>
-      </c>
-      <c r="D25" t="s">
-        <v>61</v>
-      </c>
-      <c r="E25" t="s">
-        <v>79</v>
-      </c>
-      <c r="F25" t="s">
-        <v>77</v>
-      </c>
-      <c r="G25" t="s">
-        <v>98</v>
-      </c>
-      <c r="H25">
-        <v>61</v>
-      </c>
-      <c r="J25" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A26" t="s">
-        <v>35</v>
-      </c>
-      <c r="B26" t="s">
-        <v>93</v>
-      </c>
-      <c r="C26" t="s">
-        <v>111</v>
-      </c>
-      <c r="D26" t="s">
-        <v>60</v>
-      </c>
-      <c r="E26" t="s">
-        <v>73</v>
-      </c>
-      <c r="F26" t="s">
-        <v>77</v>
-      </c>
-      <c r="G26" t="s">
-        <v>97</v>
-      </c>
-      <c r="H26">
-        <v>60</v>
-      </c>
-      <c r="J26" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A27" t="s">
-        <v>36</v>
-      </c>
-      <c r="B27" t="s">
-        <v>37</v>
-      </c>
-      <c r="C27" t="s">
-        <v>86</v>
-      </c>
-      <c r="D27" t="s">
-        <v>61</v>
-      </c>
-      <c r="E27" t="s">
-        <v>87</v>
-      </c>
-      <c r="F27" t="s">
-        <v>84</v>
-      </c>
-      <c r="G27" t="s">
-        <v>99</v>
-      </c>
-      <c r="H27">
-        <v>44</v>
-      </c>
-      <c r="J27" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A28" t="s">
-        <v>38</v>
-      </c>
-      <c r="B28" t="s">
-        <v>57</v>
-      </c>
-      <c r="C28" t="s">
-        <v>1</v>
-      </c>
-      <c r="D28" t="s">
-        <v>60</v>
-      </c>
-      <c r="E28" t="s">
-        <v>73</v>
-      </c>
-      <c r="F28" t="s">
-        <v>77</v>
-      </c>
-      <c r="G28" t="s">
-        <v>97</v>
-      </c>
-      <c r="H28">
-        <v>52</v>
-      </c>
-      <c r="J28" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A29" t="s">
-        <v>39</v>
-      </c>
-      <c r="B29" t="s">
-        <v>40</v>
-      </c>
-      <c r="C29" t="s">
-        <v>69</v>
-      </c>
-      <c r="D29" t="s">
-        <v>61</v>
-      </c>
-      <c r="E29" t="s">
-        <v>83</v>
-      </c>
-      <c r="F29" t="s">
-        <v>84</v>
-      </c>
-      <c r="G29" t="s">
-        <v>95</v>
-      </c>
-      <c r="H29">
-        <v>44</v>
-      </c>
-      <c r="I29">
-        <v>1</v>
-      </c>
-      <c r="J29" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A30" t="s">
-        <v>41</v>
-      </c>
-      <c r="B30" t="s">
-        <v>92</v>
-      </c>
-      <c r="C30" t="s">
-        <v>69</v>
-      </c>
-      <c r="D30" t="s">
-        <v>60</v>
-      </c>
-      <c r="E30" t="s">
-        <v>73</v>
-      </c>
-      <c r="F30" t="s">
-        <v>77</v>
-      </c>
-      <c r="G30" t="s">
-        <v>95</v>
-      </c>
-      <c r="H30">
-        <v>40</v>
-      </c>
-      <c r="I30">
-        <v>1</v>
-      </c>
-      <c r="J30" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A31" t="s">
-        <v>58</v>
-      </c>
-      <c r="B31" t="s">
-        <v>59</v>
-      </c>
-      <c r="C31" t="s">
-        <v>63</v>
-      </c>
-      <c r="D31" t="s">
-        <v>61</v>
-      </c>
-      <c r="E31" t="s">
-        <v>73</v>
-      </c>
-      <c r="F31" t="s">
-        <v>77</v>
-      </c>
-      <c r="I31">
-        <v>1</v>
-      </c>
-      <c r="J31" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A32" t="s">
-        <v>49</v>
-      </c>
-      <c r="B32" t="s">
-        <v>50</v>
-      </c>
-      <c r="C32" t="s">
-        <v>70</v>
-      </c>
-      <c r="D32" t="s">
-        <v>60</v>
-      </c>
-      <c r="E32" t="s">
-        <v>79</v>
-      </c>
-      <c r="F32" t="s">
-        <v>77</v>
-      </c>
-      <c r="G32" t="s">
-        <v>98</v>
-      </c>
-      <c r="H32">
-        <v>60</v>
-      </c>
-      <c r="J32" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A33" t="s">
-        <v>51</v>
-      </c>
-      <c r="B33" t="s">
-        <v>52</v>
-      </c>
-      <c r="C33" t="s">
-        <v>71</v>
-      </c>
-      <c r="D33" t="s">
-        <v>61</v>
-      </c>
-      <c r="E33" t="s">
-        <v>73</v>
-      </c>
-      <c r="F33" t="s">
-        <v>77</v>
-      </c>
-      <c r="G33" t="s">
-        <v>97</v>
-      </c>
-      <c r="H33">
-        <v>78</v>
-      </c>
-      <c r="I33">
-        <v>1</v>
-      </c>
-      <c r="J33" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A34" t="s">
-        <v>113</v>
-      </c>
-      <c r="J34" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A35" t="s">
-        <v>115</v>
-      </c>
-      <c r="J35" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A36" t="s">
-        <v>120</v>
-      </c>
-      <c r="J36" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A37" t="s">
-        <v>117</v>
-      </c>
-      <c r="J37" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A38" t="s">
-        <v>124</v>
-      </c>
-      <c r="J38" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A39" t="s">
-        <v>116</v>
-      </c>
-      <c r="J39" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A40" t="s">
-        <v>127</v>
-      </c>
-      <c r="J40" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A41" t="s">
-        <v>129</v>
-      </c>
-      <c r="J41" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A42" t="s">
-        <v>118</v>
-      </c>
-      <c r="J42" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A43" t="s">
-        <v>119</v>
-      </c>
-      <c r="J43" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A44" t="s">
-        <v>131</v>
-      </c>
-      <c r="J44" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A45" t="s">
-        <v>132</v>
-      </c>
-      <c r="J45" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A46" t="s">
-        <v>133</v>
-      </c>
-      <c r="J46" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A47" t="s">
-        <v>135</v>
-      </c>
-      <c r="J47" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A48" t="s">
-        <v>137</v>
-      </c>
-      <c r="J48" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A49" t="s">
-        <v>138</v>
-      </c>
-      <c r="J49" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A50" t="s">
-        <v>140</v>
-      </c>
-      <c r="J50" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A51" t="s">
-        <v>141</v>
-      </c>
-      <c r="J51" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A52" t="s">
-        <v>143</v>
-      </c>
-      <c r="J52" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A53" t="s">
-        <v>145</v>
-      </c>
-      <c r="J53" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A54" t="s">
-        <v>147</v>
-      </c>
-      <c r="J54" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A55" t="s">
-        <v>148</v>
-      </c>
-      <c r="J55" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A56" t="s">
-        <v>150</v>
-      </c>
-      <c r="J56" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A57" t="s">
-        <v>151</v>
-      </c>
-      <c r="J57" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A58" t="s">
-        <v>156</v>
-      </c>
-      <c r="J58" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A59" t="s">
-        <v>153</v>
-      </c>
-      <c r="J59" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A60" t="s">
-        <v>154</v>
-      </c>
-      <c r="J60" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A61" t="s">
-        <v>155</v>
-      </c>
-      <c r="J61" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A62" t="s">
-        <v>157</v>
-      </c>
-      <c r="J62" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A63" t="s">
-        <v>158</v>
-      </c>
-      <c r="J63" t="s">
-        <v>181</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>